<commit_message>
updated graph to read new excel columns
</commit_message>
<xml_diff>
--- a/utilities/data/network_diagram.xlsx
+++ b/utilities/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D15FFCE4-24B1-4A85-BC93-62E0C01F6909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60036EA9-780D-40D7-A7B5-07A8F33F040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="1140" windowWidth="38640" windowHeight="21840" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="60">
   <si>
     <t>CI_Type</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Rel_Type</t>
   </si>
   <si>
-    <t>Dependency</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
@@ -59,12 +56,12 @@
     <t>Depends On</t>
   </si>
   <si>
+    <t>dupumbvintp01</t>
+  </si>
+  <si>
     <t>CI_Descrip</t>
   </si>
   <si>
-    <t>some description</t>
-  </si>
-  <si>
     <t>Dependency_Descrip</t>
   </si>
   <si>
@@ -90,13 +87,142 @@
   </si>
   <si>
     <t>The servers that UPMIS depends on</t>
+  </si>
+  <si>
+    <t>Unclaimed Property Management System</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Dependency_Type</t>
+  </si>
+  <si>
+    <t>.NET</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Dependency_Name</t>
+  </si>
+  <si>
+    <t>MS SQL</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>Crystal Reports</t>
+  </si>
+  <si>
+    <t>ZHAO, DONGMEI</t>
+  </si>
+  <si>
+    <t>VEENSTRA, DEAN</t>
+  </si>
+  <si>
+    <t>GU, JIUJING</t>
+  </si>
+  <si>
+    <t>MCCOY, ERIC</t>
+  </si>
+  <si>
+    <t>Ye, Sean (Qiwei)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivappa, Guru </t>
+  </si>
+  <si>
+    <t>dupumbvintd01</t>
+  </si>
+  <si>
+    <t>dupumbvintd02</t>
+  </si>
+  <si>
+    <t>dupumbvintp02</t>
+  </si>
+  <si>
+    <t>dupumbvints01</t>
+  </si>
+  <si>
+    <t>dupumbvints02</t>
+  </si>
+  <si>
+    <t>dupumbvintt01</t>
+  </si>
+  <si>
+    <t>dupumbvintt02</t>
+  </si>
+  <si>
+    <t>dupumevextp01</t>
+  </si>
+  <si>
+    <t>dupumevextp02</t>
+  </si>
+  <si>
+    <t>dupumevextp03b</t>
+  </si>
+  <si>
+    <t>dupumevexts01</t>
+  </si>
+  <si>
+    <t>dupumevexts02</t>
+  </si>
+  <si>
+    <t>dupumevextt01</t>
+  </si>
+  <si>
+    <t>dupumevextt02</t>
+  </si>
+  <si>
+    <t>dupumevintd01</t>
+  </si>
+  <si>
+    <t>dupumivintd01</t>
+  </si>
+  <si>
+    <t>dupumivintp01</t>
+  </si>
+  <si>
+    <t>dupumivintp02</t>
+  </si>
+  <si>
+    <t>dumpumivintp03</t>
+  </si>
+  <si>
+    <t>dupumivints01</t>
+  </si>
+  <si>
+    <t>dupumivints02</t>
+  </si>
+  <si>
+    <t>dupumivintt01</t>
+  </si>
+  <si>
+    <t>dupumivintt02</t>
+  </si>
+  <si>
+    <t>dupumivintt03</t>
+  </si>
+  <si>
+    <t>dupvbsvintp01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +232,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -133,16 +266,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,127 +623,1012 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE7C4D-C8B9-4B8F-A7A2-DA0855C731E6}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.06640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.06640625" customWidth="1"/>
-    <col min="6" max="6" width="32.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.46484375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="33.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.53125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="32.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
showing 3 levels of nodes
</commit_message>
<xml_diff>
--- a/utilities/data/network_diagram.xlsx
+++ b/utilities/data/network_diagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B6A05C-11FF-4781-A5FC-C953F9304786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50708CC9-9226-42C1-B620-81764F5C8140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="1140" windowWidth="38640" windowHeight="21840" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="76">
   <si>
     <t>CI_Type</t>
   </si>
@@ -98,149 +98,179 @@
     <t>Dependency_Type</t>
   </si>
   <si>
-    <t>.NET</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Dependency_Name</t>
+  </si>
+  <si>
+    <t>GU, JIUJING</t>
+  </si>
+  <si>
+    <t>MCCOY, ERIC</t>
+  </si>
+  <si>
+    <t>Ye, Sean (Qiwei)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivappa, Guru </t>
+  </si>
+  <si>
+    <t>dupumbvintd01</t>
+  </si>
+  <si>
+    <t>dupumbvintd02</t>
+  </si>
+  <si>
+    <t>dupumbvintp02</t>
+  </si>
+  <si>
+    <t>dupumbvints01</t>
+  </si>
+  <si>
+    <t>dupumbvints02</t>
+  </si>
+  <si>
+    <t>dupumbvintt01</t>
+  </si>
+  <si>
+    <t>dupumbvintt02</t>
+  </si>
+  <si>
+    <t>dupumevextp01</t>
+  </si>
+  <si>
+    <t>dupumevextp02</t>
+  </si>
+  <si>
+    <t>dupumevextp03b</t>
+  </si>
+  <si>
+    <t>dupumevexts01</t>
+  </si>
+  <si>
+    <t>dupumevexts02</t>
+  </si>
+  <si>
+    <t>dupumevextt01</t>
+  </si>
+  <si>
+    <t>dupumevextt02</t>
+  </si>
+  <si>
+    <t>dupumevintd01</t>
+  </si>
+  <si>
+    <t>dupumivintd01</t>
+  </si>
+  <si>
+    <t>dupumivintp01</t>
+  </si>
+  <si>
+    <t>dupumivintp02</t>
+  </si>
+  <si>
+    <t>dumpumivintp03</t>
+  </si>
+  <si>
+    <t>dupumivints01</t>
+  </si>
+  <si>
+    <t>dupumivints02</t>
+  </si>
+  <si>
+    <t>dupumivintt01</t>
+  </si>
+  <si>
+    <t>dupumivintt02</t>
+  </si>
+  <si>
+    <t>dupumivintt03</t>
+  </si>
+  <si>
+    <t>dupvbsvintp01</t>
+  </si>
+  <si>
+    <t>Description…</t>
+  </si>
+  <si>
+    <t>FLAIR</t>
+  </si>
+  <si>
+    <t>FCDICE</t>
+  </si>
+  <si>
     <t>Java</t>
   </si>
   <si>
+    <t>A widely-used, platform-independent, object-oriented programming language designed for portability and scalability, commonly used for backend systems, Android development, and enterprise applications.</t>
+  </si>
+  <si>
     <t>C#</t>
   </si>
   <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>Dependency_Name</t>
+    <t>A modern, object-oriented programming language developed by Microsoft, primarily used for building applications within the .NET framework, including web, desktop, and game development.</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>A powerful and widely-used relational database management system (RDBMS) developed by Oracle Corporation. It supports complex queries, large-scale data storage, and enterprise-level applications, often used in businesses for high-performance database solutions, including cloud and on-premise environments.</t>
   </si>
   <si>
     <t>MS SQL</t>
   </si>
   <si>
-    <t>Oracle</t>
+    <t>(Microsoft SQL Server): A relational database management system developed by Microsoft, used for storing, retrieving, and managing data in enterprise applications.</t>
   </si>
   <si>
     <t>Crystal Reports</t>
   </si>
   <si>
-    <t>ZHAO, DONGMEI</t>
-  </si>
-  <si>
-    <t>VEENSTRA, DEAN</t>
-  </si>
-  <si>
-    <t>GU, JIUJING</t>
-  </si>
-  <si>
-    <t>MCCOY, ERIC</t>
-  </si>
-  <si>
-    <t>Ye, Sean (Qiwei)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shivappa, Guru </t>
-  </si>
-  <si>
-    <t>dupumbvintd01</t>
-  </si>
-  <si>
-    <t>dupumbvintd02</t>
-  </si>
-  <si>
-    <t>dupumbvintp02</t>
-  </si>
-  <si>
-    <t>dupumbvints01</t>
-  </si>
-  <si>
-    <t>dupumbvints02</t>
-  </si>
-  <si>
-    <t>dupumbvintt01</t>
-  </si>
-  <si>
-    <t>dupumbvintt02</t>
-  </si>
-  <si>
-    <t>dupumevextp01</t>
-  </si>
-  <si>
-    <t>dupumevextp02</t>
-  </si>
-  <si>
-    <t>dupumevextp03b</t>
-  </si>
-  <si>
-    <t>dupumevexts01</t>
-  </si>
-  <si>
-    <t>dupumevexts02</t>
-  </si>
-  <si>
-    <t>dupumevextt01</t>
-  </si>
-  <si>
-    <t>dupumevextt02</t>
-  </si>
-  <si>
-    <t>dupumevintd01</t>
-  </si>
-  <si>
-    <t>dupumivintd01</t>
-  </si>
-  <si>
-    <t>dupumivintp01</t>
-  </si>
-  <si>
-    <t>dupumivintp02</t>
-  </si>
-  <si>
-    <t>dumpumivintp03</t>
-  </si>
-  <si>
-    <t>dupumivints01</t>
-  </si>
-  <si>
-    <t>dupumivints02</t>
-  </si>
-  <si>
-    <t>dupumivintt01</t>
-  </si>
-  <si>
-    <t>dupumivintt02</t>
-  </si>
-  <si>
-    <t>dupumivintt03</t>
-  </si>
-  <si>
-    <t>dupvbsvintp01</t>
-  </si>
-  <si>
-    <t>A software development framework created by Microsoft, supporting the building and running of applications across multiple platforms. It is commonly used for web, desktop, and cloud applications.</t>
-  </si>
-  <si>
-    <t>A widely-used, platform-independent, object-oriented programming language designed for portability and scalability, commonly used for backend systems, Android development, and enterprise applications.</t>
-  </si>
-  <si>
-    <t>A modern, object-oriented programming language developed by Microsoft, primarily used for building applications within the .NET framework, including web, desktop, and game development.</t>
-  </si>
-  <si>
-    <t>(Microsoft SQL Server): A relational database management system developed by Microsoft, used for storing, retrieving, and managing data in enterprise applications.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> A business intelligence tool used to design and generate interactive and formatted reports from a wide range of data sources, often used with MS SQL Server for reporting purposes.</t>
   </si>
   <si>
-    <t>A powerful and widely-used relational database management system (RDBMS) developed by Oracle Corporation. It supports complex queries, large-scale data storage, and enterprise-level applications, often used in businesses for high-performance database solutions, including cloud and on-premise environments.</t>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Description..</t>
+  </si>
+  <si>
+    <t>ALIS</t>
+  </si>
+  <si>
+    <t>EMILI</t>
+  </si>
+  <si>
+    <t>CCAS</t>
+  </si>
+  <si>
+    <t>LSOP</t>
+  </si>
+  <si>
+    <t>AIMS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +289,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,22 +320,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,17 +674,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE7C4D-C8B9-4B8F-A7A2-DA0855C731E6}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.46484375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="44.06640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="56.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.53125" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.53125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.46484375" style="3" customWidth="1"/>
@@ -670,274 +710,250 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="57" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
@@ -946,10 +962,10 @@
         <v>21</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -957,22 +973,22 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -980,22 +996,22 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -1003,22 +1019,22 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1026,623 +1042,831 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>21</v>
+      <c r="C46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>